<commit_message>
Update RE2 engine: 2025-08-05.
</commit_message>
<xml_diff>
--- a/RegExpressWPFNET/Tools/ExportFeatureMatrix/RegexFeatureMatrix.xlsx
+++ b/RegExpressWPFNET/Tools/ExportFeatureMatrix/RegexFeatureMatrix.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Feature Matrix" sheetId="1" r:id="R83d8d881ea7949b0"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Feature Matrix" sheetId="1" r:id="R83464f1c410e4151"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -22,8 +22,8 @@
     <x:t>Description</x:t>
   </x:si>
   <x:si>
-    <x:t>Regex, .NET
-9.0.7</x:t>
+    <x:t>.NET
+9.0.8</x:t>
   </x:si>
   <x:si>
     <x:t>std::wregex
@@ -31,7 +31,7 @@
   </x:si>
   <x:si>
     <x:t>RE2
-2025-06-26</x:t>
+2025-08-05</x:t>
   </x:si>
   <x:si>
     <x:t>SubReg
@@ -261,13 +261,13 @@
     <x:t>#comment</x:t>
   </x:si>
   <x:si>
-    <x:t>Comment when enabled by options</x:t>
+    <x:t>Comment</x:t>
   </x:si>
   <x:si>
     <x:t>[#comment]</x:t>
   </x:si>
   <x:si>
-    <x:t>Comment inside […] when enabled by options</x:t>
+    <x:t>Comment inside […]</x:t>
   </x:si>
   <x:si>
     <x:t>(?flags)</x:t>
@@ -531,7 +531,7 @@
     <x:t>.</x:t>
   </x:si>
   <x:si>
-    <x:t>Any, including or excepting newline (\n) depending on options</x:t>
+    <x:t>Any, including or excepting newline (\n)</x:t>
   </x:si>
   <x:si>
     <x:t>\C</x:t>
@@ -762,13 +762,13 @@
     <x:t>^</x:t>
   </x:si>
   <x:si>
-    <x:t>Beginning of string or line, depending on options</x:t>
+    <x:t>Beginning of string or line</x:t>
   </x:si>
   <x:si>
     <x:t>$</x:t>
   </x:si>
   <x:si>
-    <x:t>End, or before '\n' at end of string or line, depending on options</x:t>
+    <x:t>End, or before '\n' at end of string or line</x:t>
   </x:si>
   <x:si>
     <x:t>\A</x:t>
@@ -858,7 +858,7 @@
     <x:t>(?@…)</x:t>
   </x:si>
   <x:si>
-    <x:t>Capturing group, depending on options</x:t>
+    <x:t>Capturing group</x:t>
   </x:si>
   <x:si>
     <x:t>\1, \2, …, \9</x:t>
@@ -930,7 +930,7 @@
     <x:t>\k&lt; … &gt;, \g&lt; … &gt;</x:t>
   </x:si>
   <x:si>
-    <x:t>Allow spaces like '\k &lt; name &gt;' when whitespaces are enabled by options</x:t>
+    <x:t>Allow spaces like '\k &lt; name &gt;'</x:t>
   </x:si>
   <x:si>
     <x:t>Grouping</x:t>
@@ -999,7 +999,7 @@
     <x:t>( ? … )</x:t>
   </x:si>
   <x:si>
-    <x:t>Allow spaces like '( ? &lt; name &gt;…)' when whitespaces are enabled by options</x:t>
+    <x:t>Allow spaces like '( ? &lt; name &gt;…)'</x:t>
   </x:si>
   <x:si>
     <x:t>Recursive patterns</x:t>
@@ -1074,9 +1074,6 @@
     <x:t>Allow spaces within {…} or \{…\}</x:t>
   </x:si>
   <x:si>
-    <x:t>Allow spaces within {…} or \{…\} when spaces are allowed by options</x:t>
-  </x:si>
-  <x:si>
     <x:t>{,m}, \{,m\}</x:t>
   </x:si>
   <x:si>
@@ -1086,7 +1083,7 @@
     <x:t>{expr}, \{expr\}</x:t>
   </x:si>
   <x:si>
-    <x:t>Approximate matching using given engine-specific expression</x:t>
+    <x:t>Approximate matching</x:t>
   </x:si>
   <x:si>
     <x:t>Conditionals</x:t>
@@ -1174,9 +1171,6 @@
   </x:si>
   <x:si>
     <x:t>(? )</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Empty construct when whitespaces are enabled by options</x:t>
   </x:si>
   <x:si>
     <x:t>[]</x:t>
@@ -1319,8 +1313,9 @@
     </x:sheetView>
   </x:sheetViews>
   <x:cols>
-    <x:col min="1" max="2" width="20" customWidth="1"/>
-    <x:col min="3" max="3" width="12.292" customWidth="1"/>
+    <x:col min="1" max="1" width="20" customWidth="1"/>
+    <x:col min="2" max="2" width="40" customWidth="1"/>
+    <x:col min="3" max="3" width="6.095" customWidth="1"/>
     <x:col min="4" max="4" width="11.789" customWidth="1"/>
     <x:col min="5" max="5" width="6.198" customWidth="1"/>
     <x:col min="6" max="6" width="9.4" customWidth="1"/>
@@ -32089,7 +32084,7 @@
         <x:v>346</x:v>
       </x:c>
       <x:c r="B184" s="5" t="s">
-        <x:v>348</x:v>
+        <x:v>347</x:v>
       </x:c>
       <x:c r="C184" t="s">
         <x:v>1</x:v>
@@ -32265,10 +32260,10 @@
     </x:row>
     <x:row r="185">
       <x:c r="A185" s="4" t="s">
+        <x:v>348</x:v>
+      </x:c>
+      <x:c r="B185" s="5" t="s">
         <x:v>349</x:v>
-      </x:c>
-      <x:c r="B185" s="5" t="s">
-        <x:v>350</x:v>
       </x:c>
       <x:c r="C185" t="s">
         <x:v>1</x:v>
@@ -32444,10 +32439,10 @@
     </x:row>
     <x:row r="186">
       <x:c r="A186" s="4" t="s">
+        <x:v>350</x:v>
+      </x:c>
+      <x:c r="B186" s="5" t="s">
         <x:v>351</x:v>
-      </x:c>
-      <x:c r="B186" s="5" t="s">
-        <x:v>352</x:v>
       </x:c>
       <x:c r="C186" t="s">
         <x:v>1</x:v>
@@ -32623,7 +32618,7 @@
     </x:row>
     <x:row r="187">
       <x:c r="A187" s="3" t="s">
-        <x:v>353</x:v>
+        <x:v>352</x:v>
       </x:c>
       <x:c r="BG187" t="s">
         <x:v>1</x:v>
@@ -32631,10 +32626,10 @@
     </x:row>
     <x:row r="188">
       <x:c r="A188" s="4" t="s">
+        <x:v>353</x:v>
+      </x:c>
+      <x:c r="B188" s="5" t="s">
         <x:v>354</x:v>
-      </x:c>
-      <x:c r="B188" s="5" t="s">
-        <x:v>355</x:v>
       </x:c>
       <x:c r="C188" s="6" t="s">
         <x:v>64</x:v>
@@ -32810,10 +32805,10 @@
     </x:row>
     <x:row r="189">
       <x:c r="A189" s="4" t="s">
+        <x:v>355</x:v>
+      </x:c>
+      <x:c r="B189" s="5" t="s">
         <x:v>356</x:v>
-      </x:c>
-      <x:c r="B189" s="5" t="s">
-        <x:v>357</x:v>
       </x:c>
       <x:c r="C189" s="6" t="s">
         <x:v>64</x:v>
@@ -32989,10 +32984,10 @@
     </x:row>
     <x:row r="190">
       <x:c r="A190" s="4" t="s">
+        <x:v>357</x:v>
+      </x:c>
+      <x:c r="B190" s="5" t="s">
         <x:v>358</x:v>
-      </x:c>
-      <x:c r="B190" s="5" t="s">
-        <x:v>359</x:v>
       </x:c>
       <x:c r="C190" s="6" t="s">
         <x:v>64</x:v>
@@ -33168,10 +33163,10 @@
     </x:row>
     <x:row r="191">
       <x:c r="A191" s="4" t="s">
+        <x:v>359</x:v>
+      </x:c>
+      <x:c r="B191" s="5" t="s">
         <x:v>360</x:v>
-      </x:c>
-      <x:c r="B191" s="5" t="s">
-        <x:v>361</x:v>
       </x:c>
       <x:c r="C191" s="6" t="s">
         <x:v>64</x:v>
@@ -33347,10 +33342,10 @@
     </x:row>
     <x:row r="192">
       <x:c r="A192" s="4" t="s">
-        <x:v>362</x:v>
+        <x:v>361</x:v>
       </x:c>
       <x:c r="B192" s="5" t="s">
-        <x:v>357</x:v>
+        <x:v>356</x:v>
       </x:c>
       <x:c r="C192" t="s">
         <x:v>1</x:v>
@@ -33526,10 +33521,10 @@
     </x:row>
     <x:row r="193">
       <x:c r="A193" s="4" t="s">
-        <x:v>363</x:v>
+        <x:v>362</x:v>
       </x:c>
       <x:c r="B193" s="5" t="s">
-        <x:v>357</x:v>
+        <x:v>356</x:v>
       </x:c>
       <x:c r="C193" t="s">
         <x:v>1</x:v>
@@ -33705,10 +33700,10 @@
     </x:row>
     <x:row r="194">
       <x:c r="A194" s="4" t="s">
+        <x:v>363</x:v>
+      </x:c>
+      <x:c r="B194" s="5" t="s">
         <x:v>364</x:v>
-      </x:c>
-      <x:c r="B194" s="5" t="s">
-        <x:v>365</x:v>
       </x:c>
       <x:c r="C194" t="s">
         <x:v>1</x:v>
@@ -33884,10 +33879,10 @@
     </x:row>
     <x:row r="195">
       <x:c r="A195" s="4" t="s">
+        <x:v>365</x:v>
+      </x:c>
+      <x:c r="B195" s="5" t="s">
         <x:v>366</x:v>
-      </x:c>
-      <x:c r="B195" s="5" t="s">
-        <x:v>367</x:v>
       </x:c>
       <x:c r="C195" t="s">
         <x:v>1</x:v>
@@ -34063,10 +34058,10 @@
     </x:row>
     <x:row r="196">
       <x:c r="A196" s="4" t="s">
+        <x:v>367</x:v>
+      </x:c>
+      <x:c r="B196" s="5" t="s">
         <x:v>368</x:v>
-      </x:c>
-      <x:c r="B196" s="5" t="s">
-        <x:v>369</x:v>
       </x:c>
       <x:c r="C196" t="s">
         <x:v>1</x:v>
@@ -34242,10 +34237,10 @@
     </x:row>
     <x:row r="197">
       <x:c r="A197" s="4" t="s">
+        <x:v>369</x:v>
+      </x:c>
+      <x:c r="B197" s="5" t="s">
         <x:v>370</x:v>
-      </x:c>
-      <x:c r="B197" s="5" t="s">
-        <x:v>371</x:v>
       </x:c>
       <x:c r="C197" t="s">
         <x:v>1</x:v>
@@ -34421,7 +34416,7 @@
     </x:row>
     <x:row r="198">
       <x:c r="A198" s="3" t="s">
-        <x:v>372</x:v>
+        <x:v>371</x:v>
       </x:c>
       <x:c r="BG198" t="s">
         <x:v>1</x:v>
@@ -34429,10 +34424,10 @@
     </x:row>
     <x:row r="199">
       <x:c r="A199" s="4" t="s">
+        <x:v>372</x:v>
+      </x:c>
+      <x:c r="B199" s="5" t="s">
         <x:v>373</x:v>
-      </x:c>
-      <x:c r="B199" s="5" t="s">
-        <x:v>374</x:v>
       </x:c>
       <x:c r="C199" t="s">
         <x:v>1</x:v>
@@ -34608,10 +34603,10 @@
     </x:row>
     <x:row r="200">
       <x:c r="A200" s="4" t="s">
+        <x:v>374</x:v>
+      </x:c>
+      <x:c r="B200" s="5" t="s">
         <x:v>375</x:v>
-      </x:c>
-      <x:c r="B200" s="5" t="s">
-        <x:v>376</x:v>
       </x:c>
       <x:c r="C200" t="s">
         <x:v>1</x:v>
@@ -34787,10 +34782,10 @@
     </x:row>
     <x:row r="201">
       <x:c r="A201" s="4" t="s">
+        <x:v>376</x:v>
+      </x:c>
+      <x:c r="B201" s="5" t="s">
         <x:v>377</x:v>
-      </x:c>
-      <x:c r="B201" s="5" t="s">
-        <x:v>378</x:v>
       </x:c>
       <x:c r="C201" t="s">
         <x:v>1</x:v>
@@ -34966,10 +34961,10 @@
     </x:row>
     <x:row r="202">
       <x:c r="A202" s="4" t="s">
+        <x:v>378</x:v>
+      </x:c>
+      <x:c r="B202" s="5" t="s">
         <x:v>379</x:v>
-      </x:c>
-      <x:c r="B202" s="5" t="s">
-        <x:v>380</x:v>
       </x:c>
       <x:c r="C202" t="s">
         <x:v>1</x:v>
@@ -35145,10 +35140,10 @@
     </x:row>
     <x:row r="203">
       <x:c r="A203" s="4" t="s">
-        <x:v>381</x:v>
+        <x:v>380</x:v>
       </x:c>
       <x:c r="B203" s="5" t="s">
-        <x:v>382</x:v>
+        <x:v>379</x:v>
       </x:c>
       <x:c r="C203" t="s">
         <x:v>1</x:v>
@@ -35324,10 +35319,10 @@
     </x:row>
     <x:row r="204">
       <x:c r="A204" s="4" t="s">
-        <x:v>383</x:v>
+        <x:v>381</x:v>
       </x:c>
       <x:c r="B204" s="5" t="s">
-        <x:v>384</x:v>
+        <x:v>382</x:v>
       </x:c>
       <x:c r="C204" t="s">
         <x:v>1</x:v>
@@ -35503,10 +35498,10 @@
     </x:row>
     <x:row r="205">
       <x:c r="A205" s="4" t="s">
-        <x:v>385</x:v>
+        <x:v>383</x:v>
       </x:c>
       <x:c r="B205" s="5" t="s">
-        <x:v>386</x:v>
+        <x:v>384</x:v>
       </x:c>
       <x:c r="C205" s="6" t="s">
         <x:v>64</x:v>

</xml_diff>